<commit_message>
[add] train eval time
</commit_message>
<xml_diff>
--- a/Nvidia GPUs对比.xlsx
+++ b/Nvidia GPUs对比.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="规格" sheetId="1" r:id="rId1"/>
-    <sheet name="对比" sheetId="2" r:id="rId2"/>
-    <sheet name="GPU 性能" sheetId="4" r:id="rId3"/>
-    <sheet name="Ref" sheetId="3" r:id="rId4"/>
+    <sheet name="GPU 性能" sheetId="4" r:id="rId2"/>
+    <sheet name="对比" sheetId="2" r:id="rId3"/>
+    <sheet name="Titan V vs RTX 2080 Ti" sheetId="5" r:id="rId4"/>
+    <sheet name="Ref" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="133">
   <si>
     <t>RTX-OPS</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -465,22 +466,92 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://www.nvidia.com/content/dam/en-zz/Solutions/design-visualization/technologies/turing-architecture/NVIDIA-Turing-Architecture-Whitepaper.pdf</t>
-  </si>
-  <si>
-    <t>http://images.nvidia.com/content/volta-architecture/pdf/volta-architecture-whitepaper.pdf</t>
-  </si>
-  <si>
-    <t>https://devblogs.nvidia.com/nvidia-turing-architecture-in-depth/</t>
-  </si>
-  <si>
-    <t>https://www.nvidia.com/en-us/titan/titan-v/</t>
-  </si>
-  <si>
-    <t>https://www.evolife.cn/computer/120761.html</t>
-  </si>
-  <si>
-    <t>http://blog.sina.com.cn/s/blog_17389e7660102y9vo.html</t>
+    <t>基础频率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1350 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1515 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显存频率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>850 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1405 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1426 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1417 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1251 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1750 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200 MHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://dawn.cs.stanford.edu/benchmark/ImageNet/train.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTX 2080Ti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Titan V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VGG 16 train</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VGG 16 eval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResNet152 train</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResNet152 eval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -644,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -684,9 +755,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -770,7 +838,373 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.7056437464033573E-2"/>
+          <c:y val="1.5985644230620485E-2"/>
+          <c:w val="0.84288708296489678"/>
+          <c:h val="0.90529358682816907"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Titan V vs RTX 2080 Ti'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RTX 2080Ti</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Titan V vs RTX 2080 Ti'!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>VGG 16 train</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VGG 16 eval</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet152 train</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ResNet152 eval</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Titan V vs RTX 2080 Ti'!$B$2:$E$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>78.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Titan V vs RTX 2080 Ti'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Titan V</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Titan V vs RTX 2080 Ti'!$B$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>VGG 16 train</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VGG 16 eval</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>ResNet152 train</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ResNet152 eval</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Titan V vs RTX 2080 Ti'!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="250"/>
+        <c:overlap val="-16"/>
+        <c:axId val="90310144"/>
+        <c:axId val="90358912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="90310144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90358912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="90358912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="90310144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>665559</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>46918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="47625"/>
+          <a:ext cx="9533334" cy="5657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>287637</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>65981</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="114300" y="5886450"/>
+          <a:ext cx="9774537" cy="5495231"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>303584</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>75509</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="11515725"/>
+          <a:ext cx="9733334" cy="5533334"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>160724</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>37418</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="图片 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="17211675"/>
+          <a:ext cx="9609524" cy="5457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1003,166 +1437,44 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>665559</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>46918</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="47625" y="47625"/>
-          <a:ext cx="9533334" cy="5657143"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>287637</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>65981</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="图片 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="114300" y="5886450"/>
-          <a:ext cx="9774537" cy="5495231"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>303584</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>75509</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="图片 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="171450" y="11515725"/>
-          <a:ext cx="9733334" cy="5533334"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>160724</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>37418</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="图片 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="152400" y="17211675"/>
-          <a:ext cx="9609524" cy="5457143"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A1:F17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
-  <autoFilter ref="A1:F17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A1:F19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="A1:F19"/>
   <tableColumns count="6">
     <tableColumn id="1" name="型号_x000a_规格" dataDxfId="5"/>
     <tableColumn id="2" name="GEFORCE RTX 2080" dataDxfId="4"/>
@@ -1462,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1532,337 +1844,383 @@
       <c r="D3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15" t="s">
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="15" t="s">
-        <v>26</v>
+        <v>114</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>120</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>42</v>
+        <v>115</v>
       </c>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="15" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="C10" s="3">
-        <v>7.5</v>
-      </c>
-      <c r="D10" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="E10" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="F10" s="11">
-        <v>7</v>
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
-        <v>66</v>
+      <c r="A11" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="F12" s="11">
+        <v>7</v>
+      </c>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="15" t="s">
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="27" x14ac:dyDescent="0.15">
-      <c r="A14" s="15" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="27" x14ac:dyDescent="0.15">
+      <c r="A16" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B16" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="8"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="26" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="22" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" s="8"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="26" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-    </row>
-    <row r="27" spans="1:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A26:F27"/>
+    <mergeCell ref="A28:F29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1875,9 +2233,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A137:K137"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A137" sqref="A137:K137"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A137" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="B137" s="22"/>
+      <c r="C137" s="22"/>
+      <c r="D137" s="22"/>
+      <c r="E137" s="22"/>
+      <c r="F137" s="22"/>
+      <c r="G137" s="22"/>
+      <c r="H137" s="22"/>
+      <c r="I137" s="22"/>
+      <c r="J137" s="22"/>
+      <c r="K137" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A137:K137"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
@@ -1889,42 +2282,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="30" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
@@ -2580,47 +2973,92 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A137:K137"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137:K137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A137" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="B137" s="23"/>
-      <c r="C137" s="23"/>
-      <c r="D137" s="23"/>
-      <c r="E137" s="23"/>
-      <c r="F137" s="23"/>
-      <c r="G137" s="23"/>
-      <c r="H137" s="23"/>
-      <c r="I137" s="23"/>
-      <c r="J137" s="23"/>
-      <c r="K137" s="23"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="C2">
+        <v>23.6</v>
+      </c>
+      <c r="D2">
+        <v>178</v>
+      </c>
+      <c r="E2">
+        <v>37.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B3">
+        <v>82.5</v>
+      </c>
+      <c r="C3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D3">
+        <v>52.7</v>
+      </c>
+      <c r="E3">
+        <v>29.1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A137:K137"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2723,34 +3161,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A20" s="21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A21" s="21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A22" s="21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A23" s="21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A24" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A25" s="14" t="s">
-        <v>116</v>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A20" s="14" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2775,13 +3188,7 @@
     <hyperlink ref="A18" r:id="rId17"/>
     <hyperlink ref="A19" r:id="rId18"/>
     <hyperlink ref="A20" r:id="rId19"/>
-    <hyperlink ref="A21" r:id="rId20"/>
-    <hyperlink ref="A22" r:id="rId21"/>
-    <hyperlink ref="A23" r:id="rId22"/>
-    <hyperlink ref="A24" r:id="rId23"/>
-    <hyperlink ref="A25" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>